<commit_message>
mapping turtle and rdfxml
</commit_message>
<xml_diff>
--- a/data/source/provenanceweb/file-format-mappings/version/latest/source/file-format-mappings.xlsx
+++ b/data/source/provenanceweb/file-format-mappings/version/latest/source/file-format-mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="500"/>
+    <workbookView xWindow="10720" yWindow="0" windowWidth="17400" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>formats/pronom/x-fmt/18</t>
   </si>
@@ -31,16 +31,42 @@
   </si>
   <si>
     <t>format/mime/text/csv</t>
+  </si>
+  <si>
+    <t>format/mime/text/turtle</t>
+  </si>
+  <si>
+    <t>W3C</t>
+  </si>
+  <si>
+    <t>Turtle</t>
+  </si>
+  <si>
+    <t>RDF_XML</t>
+  </si>
+  <si>
+    <t>format/mime/application/rdf+xml</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,13 +89,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,36 +427,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>